<commit_message>
fix transaksi stok, login, report
</commit_message>
<xml_diff>
--- a/logicku.xlsx
+++ b/logicku.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\salesmotoris\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D752621-C9A5-4E42-AE32-9F1C89DFD2C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{143A4B28-0B27-4076-806B-3A3ABB7428C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4005" yWindow="1260" windowWidth="11520" windowHeight="7875" xr2:uid="{D36B6A87-A639-4DB4-B01C-9F5223CD2069}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D36B6A87-A639-4DB4-B01C-9F5223CD2069}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>perbulan</t>
   </si>
@@ -63,6 +64,12 @@
   </si>
   <si>
     <t>//add to date</t>
+  </si>
+  <si>
+    <t>target sisa</t>
+  </si>
+  <si>
+    <t>trg tmbh</t>
   </si>
 </sst>
 </file>
@@ -417,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89A68AFF-8B53-499C-B087-46A6C0B9C40E}">
-  <dimension ref="B2:H17"/>
+  <dimension ref="B2:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,7 +437,7 @@
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -443,65 +450,96 @@
       <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1">
-        <v>60</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
       </c>
       <c r="F3" s="1">
-        <f>C3/30</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G3" s="1">
-        <v>1</v>
-      </c>
-      <c r="H3" s="1">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="J3" s="1">
+        <v>60</v>
+      </c>
+      <c r="K3" s="1">
+        <v>17</v>
+      </c>
+      <c r="M3" s="1">
+        <v>3</v>
+      </c>
+      <c r="N3" s="1">
+        <v>3</v>
+      </c>
+      <c r="O3" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" s="1">
         <v>2</v>
       </c>
       <c r="F4" s="1">
-        <f>C3/30+(F3-G3)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G4" s="1">
         <v>1</v>
       </c>
       <c r="H4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+        <f>C5-F5-F4</f>
+        <v>-8</v>
+      </c>
+      <c r="J4" s="1">
+        <f>J3/K3</f>
+        <v>3.5294117647058822</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1">
+        <f>C3-G6</f>
+        <v>-1</v>
+      </c>
       <c r="E5" s="1">
         <v>3</v>
       </c>
       <c r="F5" s="1">
-        <f>C3/30+(F4-G4)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G5" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+        <f>C5-F5</f>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="G6" s="1">
+        <f>SUM(G3:G5)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -509,7 +547,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C9" s="1">
         <v>1</v>
       </c>
@@ -523,37 +561,37 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C10" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C11" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C12" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C13" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C14" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C15" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C16" s="1">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
update api to remotemysql
</commit_message>
<xml_diff>
--- a/logicku.xlsx
+++ b/logicku.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\salesmotoris\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD01C54-0B51-4FED-B175-87C4A36F2F59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C7F381-8254-4B93-988D-8A0E7F9E6F84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D36B6A87-A639-4DB4-B01C-9F5223CD2069}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>perbulan</t>
   </si>
@@ -69,6 +69,27 @@
   </si>
   <si>
     <t>trg tmbh</t>
+  </si>
+  <si>
+    <t>toko</t>
+  </si>
+  <si>
+    <t>nama sales</t>
+  </si>
+  <si>
+    <t>barang</t>
+  </si>
+  <si>
+    <t>omz</t>
+  </si>
+  <si>
+    <t>agung</t>
+  </si>
+  <si>
+    <t>wafer2000c;20pcs</t>
+  </si>
+  <si>
+    <t>ec</t>
   </si>
 </sst>
 </file>
@@ -423,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89A68AFF-8B53-499C-B087-46A6C0B9C40E}">
-  <dimension ref="B2:O17"/>
+  <dimension ref="B2:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,9 +616,49 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C17" s="1">
         <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="1">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="35" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D35" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D36" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E36" s="1">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix error store, product focus
</commit_message>
<xml_diff>
--- a/logicku.xlsx
+++ b/logicku.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProgramFile\xampp\htdocs\salesmotoris\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C451484-2832-43B7-B633-A856EEDB8189}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F534C3-9C9E-4036-A0AD-EC9AFA9B542D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D36B6A87-A639-4DB4-B01C-9F5223CD2069}"/>
   </bookViews>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -74,9 +72,6 @@
     <t>toko</t>
   </si>
   <si>
-    <t>nama sales</t>
-  </si>
-  <si>
     <t>barang</t>
   </si>
   <si>
@@ -90,6 +85,9 @@
   </si>
   <si>
     <t>ec</t>
+  </si>
+  <si>
+    <t>salesman</t>
   </si>
 </sst>
 </file>
@@ -447,7 +445,7 @@
   <dimension ref="B2:O36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,33 +614,31 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C17" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="1" t="s">
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="E21" s="1">
         <v>200000</v>
@@ -650,12 +646,12 @@
     </row>
     <row r="35" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D35" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D36" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E36" s="1">
         <v>15</v>

</xml_diff>